<commit_message>
add the visual effect on trap
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SpellTrap.xlsx
+++ b/ConfigData/Xlsx/SpellTrap.xlsx
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -145,51 +145,95 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>召唤时触发</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用卡牌时触发</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>return false;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>return false;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰晶</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>爆炸陷阱</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SpellTrapSummonDelegate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对目标造成一定伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰冻召唤的怪物5回合</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>m.AddBuff(56000009,lv,5);return true;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>m.OnMagicDamage(null,t.Damage,3);return true;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰冻陷阱</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>m.Return((int)t.Help);return true;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>把目标移动回手牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>EffectSummon</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>召唤时触发</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>使用卡牌时触发</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>return false;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>return false;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>冰晶</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>爆炸陷阱</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SpellTrapSummonDelegate</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对目标造成一定伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>冰冻召唤的怪物5回合</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>m.AddBuff(56000009,lv,5);return true;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>m.OnMagicDamage(null,t.Damage,3);return true;</t>
+    <t>UnitEffect</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>特效</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>firehit</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>iceball</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>icesharp</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>silent</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>pinkball</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bluewing</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1148,17 +1192,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:E9" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
-  <autoFilter ref="A3:E9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:F10" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="A3:F10"/>
   <sortState ref="A4:Z126">
     <sortCondition ref="A3:A126"/>
   </sortState>
-  <tableColumns count="5">
+  <tableColumns count="6">
     <tableColumn id="1" name="Id" dataDxfId="4"/>
     <tableColumn id="2" name="Name" dataDxfId="3"/>
     <tableColumn id="22" name="EffectUse" dataDxfId="2"/>
     <tableColumn id="4" name="EffectSummon" dataDxfId="1"/>
     <tableColumn id="3" name="Comment" dataDxfId="0"/>
+    <tableColumn id="5" name="UnitEffect"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1451,13 +1496,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1468,7 +1513,7 @@
     <col min="5" max="5" width="49.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="65.25" customHeight="1">
+    <row r="1" spans="1:6" ht="65.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
@@ -1476,16 +1521,19 @@
         <v>5</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="F1" s="7" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1496,13 +1544,16 @@
         <v>20</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="F2" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1513,13 +1564,16 @@
         <v>21</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>14</v>
       </c>
+      <c r="F3" s="9" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" ht="36">
+    <row r="4" spans="1:6" ht="36">
       <c r="A4" s="5">
         <v>54000001</v>
       </c>
@@ -1530,13 +1584,16 @@
         <v>6</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>15</v>
       </c>
+      <c r="F4" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" ht="36">
+    <row r="5" spans="1:6" ht="36">
       <c r="A5" s="8">
         <v>54000002</v>
       </c>
@@ -1547,13 +1604,16 @@
         <v>10</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>11</v>
       </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" ht="24">
+    <row r="6" spans="1:6" ht="24">
       <c r="A6" s="8">
         <v>54000003</v>
       </c>
@@ -1564,13 +1624,16 @@
         <v>8</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>13</v>
       </c>
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" ht="24">
+    <row r="7" spans="1:6" ht="24">
       <c r="A7" s="8">
         <v>54000004</v>
       </c>
@@ -1581,44 +1644,73 @@
         <v>18</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>19</v>
       </c>
+      <c r="F7" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="8" spans="1:5" ht="24">
+    <row r="8" spans="1:6" ht="24">
       <c r="A8" s="8">
         <v>54000005</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="24">
+    <row r="9" spans="1:6" ht="24">
       <c r="A9" s="8">
         <v>54000006</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="24">
+      <c r="A10" s="8">
+        <v>54000007</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>30</v>
+      <c r="C10" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
split the PlayerAction from player with scrpit
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/SpellTrap.xlsx
+++ b/ConfigData/Xlsx/SpellTrap.xlsx
@@ -81,26 +81,14 @@
     <t>名字</t>
   </si>
   <si>
-    <t>if(type==2){r.DeleteSelectCard();return true;}return false;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>说明</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>r.DeleteSelectCard();return true;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>法术反制</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>if(type==3){r.DeleteSelectCard();return true;}return false;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>使对方使用的魔法卡破坏</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -129,10 +117,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>r.RecostSelectCard();return true;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>使对方使用的卡牌消耗额外增加1倍</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -262,6 +246,22 @@
   </si>
   <si>
     <t>m.Action.Return((int)t.Help);return true;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(type==2){r.Action.DeleteSelectCard();return true;}return false;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(type==3){r.Action.DeleteSelectCard();return true;}return false;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>r.Action.DeleteSelectCard();return true;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>r.Action.RecostSelectCard();return true;</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1600,7 +1600,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1620,19 +1620,19 @@
         <v>5</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
@@ -1643,13 +1643,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>1</v>
@@ -1666,19 +1666,19 @@
         <v>3</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="24" x14ac:dyDescent="0.15">
@@ -1686,22 +1686,22 @@
         <v>54000001</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E4" s="8">
         <v>1</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="24" x14ac:dyDescent="0.15">
@@ -1709,68 +1709,68 @@
         <v>54000002</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E5" s="8">
         <v>1</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="24" x14ac:dyDescent="0.15">
       <c r="A6" s="8">
         <v>54000003</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E6" s="8">
         <v>3</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="24" x14ac:dyDescent="0.15">
       <c r="A7" s="8">
         <v>54000004</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E7" s="8">
         <v>1</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="24" x14ac:dyDescent="0.15">
@@ -1778,22 +1778,22 @@
         <v>54000005</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E8" s="8">
         <v>1</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="24" x14ac:dyDescent="0.15">
@@ -1801,22 +1801,22 @@
         <v>54000006</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>27</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>31</v>
       </c>
       <c r="E9" s="8">
         <v>1</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="24" x14ac:dyDescent="0.15">
@@ -1824,22 +1824,22 @@
         <v>54000007</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E10" s="8">
         <v>1</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="24" x14ac:dyDescent="0.15">
@@ -1847,22 +1847,22 @@
         <v>54000008</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E11" s="8">
         <v>1</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>